<commit_message>
ignore some system components
</commit_message>
<xml_diff>
--- a/pkg-info.xlsx
+++ b/pkg-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Documents\Source Codes\gkd-rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9F82A1-ABBA-4E0C-8913-20F7BE01EB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B8D81-BE18-4081-8882-4FA8F2B4F7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$928</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$942</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1745">
   <si>
     <t>package_name</t>
   </si>
@@ -3739,9 +3739,6 @@
     <t>com.miui.virtualsim</t>
   </si>
   <si>
-    <t>虚拟SIM卡</t>
-  </si>
-  <si>
     <t>com.cnspeedtest.globalspeed</t>
   </si>
   <si>
@@ -4084,9 +4081,6 @@
     <t>com.android.contacts</t>
   </si>
   <si>
-    <t>联系人</t>
-  </si>
-  <si>
     <t>com.tongcheng.android</t>
   </si>
   <si>
@@ -4216,9 +4210,6 @@
     <t>com.android.documentsui</t>
   </si>
   <si>
-    <t>DocumentUI</t>
-  </si>
-  <si>
     <t>com.baidu.newapp</t>
   </si>
   <si>
@@ -4399,9 +4390,6 @@
     <t>com.android.browser</t>
   </si>
   <si>
-    <t>浏览器</t>
-  </si>
-  <si>
     <t>com.xiaomi.shop</t>
   </si>
   <si>
@@ -4411,9 +4399,6 @@
     <t>com.xiaomi.vipaccount</t>
   </si>
   <si>
-    <t>VIP米币</t>
-  </si>
-  <si>
     <t>com.miui.video</t>
   </si>
   <si>
@@ -4432,9 +4417,6 @@
     <t>com.xiaomi.gamecenter.sdk.service</t>
   </si>
   <si>
-    <t>游戏服务</t>
-  </si>
-  <si>
     <t>com.xiaomi.gamecenter</t>
   </si>
   <si>
@@ -4462,9 +4444,6 @@
     <t>com.xiaomi.account</t>
   </si>
   <si>
-    <t>小米帐号</t>
-  </si>
-  <si>
     <t>com.sjmly.sjmtask.xsh</t>
   </si>
   <si>
@@ -4966,9 +4945,6 @@
     <t>com.android.thememanager</t>
   </si>
   <si>
-    <t>主题</t>
-  </si>
-  <si>
     <t>com.wuba.zhuanzhuan</t>
   </si>
   <si>
@@ -5086,9 +5062,6 @@
     <t>com.google.android.gms</t>
   </si>
   <si>
-    <t>GMS</t>
-  </si>
-  <si>
     <t>com.android.vending</t>
   </si>
   <si>
@@ -5186,6 +5159,117 @@
   </si>
   <si>
     <t>Google翻译</t>
+  </si>
+  <si>
+    <t>com.jingcai.apps.qualitydev</t>
+  </si>
+  <si>
+    <t>到梦空间</t>
+  </si>
+  <si>
+    <t>com.huabenapp</t>
+  </si>
+  <si>
+    <t>话本小说</t>
+  </si>
+  <si>
+    <t>world.letsgo.booster.android.pro</t>
+  </si>
+  <si>
+    <t>com.kmsoft.fvplayer</t>
+  </si>
+  <si>
+    <t>快码万能播放器</t>
+  </si>
+  <si>
+    <t>com.github.catvod.app</t>
+  </si>
+  <si>
+    <t>com.pingan.paces.ccms</t>
+  </si>
+  <si>
+    <t>平安口袋银行</t>
+  </si>
+  <si>
+    <t>com.leiting.lt65207</t>
+  </si>
+  <si>
+    <t>com.zhouyu.music</t>
+  </si>
+  <si>
+    <t>com.sec.android.app.camera</t>
+  </si>
+  <si>
+    <t>yyc.xk</t>
+  </si>
+  <si>
+    <t>星空视频壁纸</t>
+  </si>
+  <si>
+    <t>com.cib.xyk</t>
+  </si>
+  <si>
+    <t>兴业生活</t>
+  </si>
+  <si>
+    <t>com.hihanhan.one.rt45</t>
+  </si>
+  <si>
+    <t>com.yipiao</t>
+  </si>
+  <si>
+    <t>智行火车票</t>
+  </si>
+  <si>
+    <t>com.tencent.qqlite</t>
+  </si>
+  <si>
+    <t>未知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QQ精简版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米社区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全球上网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通讯录与拨号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米浏览器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米游戏服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米账号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主题壁纸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android 系统文件选择器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Play 服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5536,10 +5620,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C928"/>
+  <dimension ref="A1:C942"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H116" sqref="H116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -6099,7 +6183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -6297,7 +6381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -7012,7 +7096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>266</v>
       </c>
@@ -7309,7 +7393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>318</v>
       </c>
@@ -7317,10 +7401,10 @@
         <v>319</v>
       </c>
       <c r="C161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>320</v>
       </c>
@@ -7328,7 +7412,7 @@
         <v>321</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
@@ -9179,7 +9263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A331" t="s">
         <v>651</v>
       </c>
@@ -9366,7 +9450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="348" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A348" t="s">
         <v>685</v>
       </c>
@@ -9509,7 +9593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A361" t="s">
         <v>710</v>
       </c>
@@ -9707,7 +9791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A379" t="s">
         <v>746</v>
       </c>
@@ -9916,7 +10000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A398" t="s">
         <v>780</v>
       </c>
@@ -9924,7 +10008,7 @@
         <v>781</v>
       </c>
       <c r="C398">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
@@ -10114,7 +10198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A416" t="s">
         <v>810</v>
       </c>
@@ -10122,7 +10206,7 @@
         <v>319</v>
       </c>
       <c r="C416">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
@@ -10829,7 +10913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="481" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A481" t="s">
         <v>929</v>
       </c>
@@ -10851,7 +10935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="483" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A483" t="s">
         <v>933</v>
       </c>
@@ -10859,7 +10943,7 @@
         <v>934</v>
       </c>
       <c r="C483">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="484" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
@@ -10906,7 +10990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="488" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A488" t="s">
         <v>943</v>
       </c>
@@ -10914,7 +10998,7 @@
         <v>944</v>
       </c>
       <c r="C488">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
@@ -10972,7 +11056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="494" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A494" t="s">
         <v>955</v>
       </c>
@@ -11588,7 +11672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="550" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="550" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A550" t="s">
         <v>1062</v>
       </c>
@@ -11698,7 +11782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="560" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="560" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A560" t="s">
         <v>1082</v>
       </c>
@@ -12699,23 +12783,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="651" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="651" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A651" t="s">
         <v>1237</v>
       </c>
       <c r="B651" t="s">
-        <v>1238</v>
+        <v>1736</v>
       </c>
       <c r="C651">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="652" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A652" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B652" t="s">
         <v>1239</v>
-      </c>
-      <c r="B652" t="s">
-        <v>1240</v>
       </c>
       <c r="C652">
         <v>1</v>
@@ -12723,10 +12807,10 @@
     </row>
     <row r="653" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A653" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B653" t="s">
         <v>1241</v>
-      </c>
-      <c r="B653" t="s">
-        <v>1242</v>
       </c>
       <c r="C653">
         <v>1</v>
@@ -12734,10 +12818,10 @@
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A654" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B654" t="s">
         <v>1243</v>
-      </c>
-      <c r="B654" t="s">
-        <v>1244</v>
       </c>
       <c r="C654">
         <v>0</v>
@@ -12745,7 +12829,7 @@
     </row>
     <row r="655" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A655" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B655" t="s">
         <v>605</v>
@@ -12756,10 +12840,10 @@
     </row>
     <row r="656" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A656" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B656" t="s">
         <v>1246</v>
-      </c>
-      <c r="B656" t="s">
-        <v>1247</v>
       </c>
       <c r="C656">
         <v>1</v>
@@ -12767,10 +12851,10 @@
     </row>
     <row r="657" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A657" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B657" t="s">
         <v>1248</v>
-      </c>
-      <c r="B657" t="s">
-        <v>1249</v>
       </c>
       <c r="C657">
         <v>1</v>
@@ -12778,10 +12862,10 @@
     </row>
     <row r="658" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A658" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B658" t="s">
         <v>1250</v>
-      </c>
-      <c r="B658" t="s">
-        <v>1251</v>
       </c>
       <c r="C658">
         <v>1</v>
@@ -12789,7 +12873,7 @@
     </row>
     <row r="659" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A659" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B659" t="s">
         <v>605</v>
@@ -12800,10 +12884,10 @@
     </row>
     <row r="660" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A660" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B660" t="s">
         <v>1253</v>
-      </c>
-      <c r="B660" t="s">
-        <v>1254</v>
       </c>
       <c r="C660">
         <v>1</v>
@@ -12811,10 +12895,10 @@
     </row>
     <row r="661" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A661" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B661" t="s">
         <v>1255</v>
-      </c>
-      <c r="B661" t="s">
-        <v>1256</v>
       </c>
       <c r="C661">
         <v>1</v>
@@ -12822,7 +12906,7 @@
     </row>
     <row r="662" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A662" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B662" t="s">
         <v>605</v>
@@ -12833,10 +12917,10 @@
     </row>
     <row r="663" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A663" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B663" t="s">
         <v>1258</v>
-      </c>
-      <c r="B663" t="s">
-        <v>1259</v>
       </c>
       <c r="C663">
         <v>1</v>
@@ -12844,10 +12928,10 @@
     </row>
     <row r="664" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A664" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B664" t="s">
         <v>1260</v>
-      </c>
-      <c r="B664" t="s">
-        <v>1261</v>
       </c>
       <c r="C664">
         <v>1</v>
@@ -12855,10 +12939,10 @@
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A665" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B665" t="s">
         <v>1262</v>
-      </c>
-      <c r="B665" t="s">
-        <v>1263</v>
       </c>
       <c r="C665">
         <v>0</v>
@@ -12866,10 +12950,10 @@
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A666" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B666" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C666">
         <v>0</v>
@@ -12877,7 +12961,7 @@
     </row>
     <row r="667" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A667" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B667" t="s">
         <v>605</v>
@@ -12888,10 +12972,10 @@
     </row>
     <row r="668" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A668" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B668" t="s">
         <v>1266</v>
-      </c>
-      <c r="B668" t="s">
-        <v>1267</v>
       </c>
       <c r="C668">
         <v>1</v>
@@ -12899,10 +12983,10 @@
     </row>
     <row r="669" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A669" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B669" t="s">
         <v>1268</v>
-      </c>
-      <c r="B669" t="s">
-        <v>1269</v>
       </c>
       <c r="C669">
         <v>1</v>
@@ -12910,10 +12994,10 @@
     </row>
     <row r="670" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A670" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B670" t="s">
         <v>1270</v>
-      </c>
-      <c r="B670" t="s">
-        <v>1271</v>
       </c>
       <c r="C670">
         <v>1</v>
@@ -12921,10 +13005,10 @@
     </row>
     <row r="671" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A671" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B671" t="s">
         <v>1272</v>
-      </c>
-      <c r="B671" t="s">
-        <v>1273</v>
       </c>
       <c r="C671">
         <v>1</v>
@@ -12932,10 +13016,10 @@
     </row>
     <row r="672" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A672" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B672" t="s">
         <v>1274</v>
-      </c>
-      <c r="B672" t="s">
-        <v>1275</v>
       </c>
       <c r="C672">
         <v>1</v>
@@ -12943,7 +13027,7 @@
     </row>
     <row r="673" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A673" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B673" t="s">
         <v>605</v>
@@ -12954,10 +13038,10 @@
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A674" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B674" t="s">
         <v>1277</v>
-      </c>
-      <c r="B674" t="s">
-        <v>1278</v>
       </c>
       <c r="C674">
         <v>0</v>
@@ -12965,21 +13049,21 @@
     </row>
     <row r="675" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A675" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B675" t="s">
         <v>1279</v>
       </c>
-      <c r="B675" t="s">
+      <c r="C675">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A676" t="s">
         <v>1280</v>
       </c>
-      <c r="C675">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="676" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A676" t="s">
+      <c r="B676" t="s">
         <v>1281</v>
-      </c>
-      <c r="B676" t="s">
-        <v>1282</v>
       </c>
       <c r="C676">
         <v>1</v>
@@ -12987,7 +13071,7 @@
     </row>
     <row r="677" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A677" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B677" t="s">
         <v>605</v>
@@ -12998,10 +13082,10 @@
     </row>
     <row r="678" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A678" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B678" t="s">
         <v>1284</v>
-      </c>
-      <c r="B678" t="s">
-        <v>1285</v>
       </c>
       <c r="C678">
         <v>1</v>
@@ -13009,7 +13093,7 @@
     </row>
     <row r="679" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A679" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B679" t="s">
         <v>605</v>
@@ -13020,10 +13104,10 @@
     </row>
     <row r="680" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A680" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B680" t="s">
         <v>1287</v>
-      </c>
-      <c r="B680" t="s">
-        <v>1288</v>
       </c>
       <c r="C680">
         <v>1</v>
@@ -13031,10 +13115,10 @@
     </row>
     <row r="681" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A681" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B681" t="s">
         <v>1289</v>
-      </c>
-      <c r="B681" t="s">
-        <v>1290</v>
       </c>
       <c r="C681">
         <v>1</v>
@@ -13042,7 +13126,7 @@
     </row>
     <row r="682" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A682" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B682" t="s">
         <v>605</v>
@@ -13053,10 +13137,10 @@
     </row>
     <row r="683" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A683" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B683" t="s">
         <v>1292</v>
-      </c>
-      <c r="B683" t="s">
-        <v>1293</v>
       </c>
       <c r="C683">
         <v>1</v>
@@ -13064,10 +13148,10 @@
     </row>
     <row r="684" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A684" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B684" t="s">
         <v>1294</v>
-      </c>
-      <c r="B684" t="s">
-        <v>1295</v>
       </c>
       <c r="C684">
         <v>1</v>
@@ -13075,10 +13159,10 @@
     </row>
     <row r="685" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A685" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B685" t="s">
         <v>1296</v>
-      </c>
-      <c r="B685" t="s">
-        <v>1297</v>
       </c>
       <c r="C685">
         <v>1</v>
@@ -13086,10 +13170,10 @@
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A686" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B686" t="s">
         <v>1298</v>
-      </c>
-      <c r="B686" t="s">
-        <v>1299</v>
       </c>
       <c r="C686">
         <v>0</v>
@@ -13097,10 +13181,10 @@
     </row>
     <row r="687" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A687" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B687" t="s">
         <v>1300</v>
-      </c>
-      <c r="B687" t="s">
-        <v>1301</v>
       </c>
       <c r="C687">
         <v>1</v>
@@ -13108,10 +13192,10 @@
     </row>
     <row r="688" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A688" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B688" t="s">
         <v>1302</v>
-      </c>
-      <c r="B688" t="s">
-        <v>1303</v>
       </c>
       <c r="C688">
         <v>1</v>
@@ -13119,10 +13203,10 @@
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A689" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B689" t="s">
         <v>1304</v>
-      </c>
-      <c r="B689" t="s">
-        <v>1305</v>
       </c>
       <c r="C689">
         <v>0</v>
@@ -13130,10 +13214,10 @@
     </row>
     <row r="690" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A690" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B690" t="s">
         <v>1306</v>
-      </c>
-      <c r="B690" t="s">
-        <v>1307</v>
       </c>
       <c r="C690">
         <v>1</v>
@@ -13141,10 +13225,10 @@
     </row>
     <row r="691" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A691" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B691" t="s">
         <v>1308</v>
-      </c>
-      <c r="B691" t="s">
-        <v>1309</v>
       </c>
       <c r="C691">
         <v>1</v>
@@ -13152,7 +13236,7 @@
     </row>
     <row r="692" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A692" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B692" t="s">
         <v>605</v>
@@ -13163,7 +13247,7 @@
     </row>
     <row r="693" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A693" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B693" t="s">
         <v>605</v>
@@ -13174,7 +13258,7 @@
     </row>
     <row r="694" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A694" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B694" t="s">
         <v>605</v>
@@ -13185,10 +13269,10 @@
     </row>
     <row r="695" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A695" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B695" t="s">
         <v>1313</v>
-      </c>
-      <c r="B695" t="s">
-        <v>1314</v>
       </c>
       <c r="C695">
         <v>1</v>
@@ -13196,10 +13280,10 @@
     </row>
     <row r="696" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A696" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B696" t="s">
         <v>1315</v>
-      </c>
-      <c r="B696" t="s">
-        <v>1316</v>
       </c>
       <c r="C696">
         <v>1</v>
@@ -13207,7 +13291,7 @@
     </row>
     <row r="697" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A697" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B697" t="s">
         <v>605</v>
@@ -13218,7 +13302,7 @@
     </row>
     <row r="698" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A698" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B698" t="s">
         <v>605</v>
@@ -13229,10 +13313,10 @@
     </row>
     <row r="699" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A699" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B699" t="s">
         <v>1319</v>
-      </c>
-      <c r="B699" t="s">
-        <v>1320</v>
       </c>
       <c r="C699">
         <v>1</v>
@@ -13240,10 +13324,10 @@
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A700" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B700" t="s">
         <v>1321</v>
-      </c>
-      <c r="B700" t="s">
-        <v>1322</v>
       </c>
       <c r="C700">
         <v>0</v>
@@ -13251,7 +13335,7 @@
     </row>
     <row r="701" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A701" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B701" t="s">
         <v>605</v>
@@ -13262,10 +13346,10 @@
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A702" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B702" t="s">
         <v>1324</v>
-      </c>
-      <c r="B702" t="s">
-        <v>1325</v>
       </c>
       <c r="C702">
         <v>0</v>
@@ -13273,10 +13357,10 @@
     </row>
     <row r="703" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A703" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B703" t="s">
         <v>1326</v>
-      </c>
-      <c r="B703" t="s">
-        <v>1327</v>
       </c>
       <c r="C703">
         <v>1</v>
@@ -13284,10 +13368,10 @@
     </row>
     <row r="704" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A704" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B704" t="s">
         <v>1328</v>
-      </c>
-      <c r="B704" t="s">
-        <v>1329</v>
       </c>
       <c r="C704">
         <v>1</v>
@@ -13295,10 +13379,10 @@
     </row>
     <row r="705" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A705" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B705" t="s">
         <v>1330</v>
-      </c>
-      <c r="B705" t="s">
-        <v>1331</v>
       </c>
       <c r="C705">
         <v>1</v>
@@ -13306,7 +13390,7 @@
     </row>
     <row r="706" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A706" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B706" t="s">
         <v>605</v>
@@ -13317,10 +13401,10 @@
     </row>
     <row r="707" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A707" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B707" t="s">
         <v>1333</v>
-      </c>
-      <c r="B707" t="s">
-        <v>1334</v>
       </c>
       <c r="C707">
         <v>1</v>
@@ -13328,7 +13412,7 @@
     </row>
     <row r="708" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A708" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B708" t="s">
         <v>605</v>
@@ -13339,7 +13423,7 @@
     </row>
     <row r="709" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A709" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B709" t="s">
         <v>605</v>
@@ -13350,10 +13434,10 @@
     </row>
     <row r="710" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A710" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B710" t="s">
         <v>1337</v>
-      </c>
-      <c r="B710" t="s">
-        <v>1338</v>
       </c>
       <c r="C710">
         <v>1</v>
@@ -13361,7 +13445,7 @@
     </row>
     <row r="711" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A711" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B711" t="s">
         <v>605</v>
@@ -13372,10 +13456,10 @@
     </row>
     <row r="712" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A712" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B712" t="s">
         <v>1340</v>
-      </c>
-      <c r="B712" t="s">
-        <v>1341</v>
       </c>
       <c r="C712">
         <v>1</v>
@@ -13383,10 +13467,10 @@
     </row>
     <row r="713" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A713" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B713" t="s">
         <v>1342</v>
-      </c>
-      <c r="B713" t="s">
-        <v>1343</v>
       </c>
       <c r="C713">
         <v>1</v>
@@ -13394,10 +13478,10 @@
     </row>
     <row r="714" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A714" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B714" t="s">
         <v>1344</v>
-      </c>
-      <c r="B714" t="s">
-        <v>1345</v>
       </c>
       <c r="C714">
         <v>1</v>
@@ -13405,10 +13489,10 @@
     </row>
     <row r="715" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A715" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B715" t="s">
         <v>1346</v>
-      </c>
-      <c r="B715" t="s">
-        <v>1347</v>
       </c>
       <c r="C715">
         <v>1</v>
@@ -13416,7 +13500,7 @@
     </row>
     <row r="716" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A716" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B716" t="s">
         <v>605</v>
@@ -13427,7 +13511,7 @@
     </row>
     <row r="717" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A717" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B717" t="s">
         <v>605</v>
@@ -13438,32 +13522,32 @@
     </row>
     <row r="718" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A718" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B718" t="s">
         <v>1350</v>
       </c>
-      <c r="B718" t="s">
+      <c r="C718">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A719" t="s">
         <v>1351</v>
       </c>
-      <c r="C718">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="719" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A719" t="s">
-        <v>1352</v>
-      </c>
       <c r="B719" t="s">
-        <v>1353</v>
+        <v>1737</v>
       </c>
       <c r="C719">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="720" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A720" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="B720" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C720">
         <v>1</v>
@@ -13471,10 +13555,10 @@
     </row>
     <row r="721" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A721" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B721" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="C721">
         <v>1</v>
@@ -13482,10 +13566,10 @@
     </row>
     <row r="722" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A722" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="B722" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="C722">
         <v>1</v>
@@ -13493,7 +13577,7 @@
     </row>
     <row r="723" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A723" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B723" t="s">
         <v>605</v>
@@ -13504,10 +13588,10 @@
     </row>
     <row r="724" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A724" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="B724" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C724">
         <v>1</v>
@@ -13515,10 +13599,10 @@
     </row>
     <row r="725" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A725" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="B725" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C725">
         <v>1</v>
@@ -13526,10 +13610,10 @@
     </row>
     <row r="726" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A726" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="B726" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C726">
         <v>1</v>
@@ -13537,10 +13621,10 @@
     </row>
     <row r="727" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A727" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="B727" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C727">
         <v>1</v>
@@ -13548,10 +13632,10 @@
     </row>
     <row r="728" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A728" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="B728" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="C728">
         <v>1</v>
@@ -13559,10 +13643,10 @@
     </row>
     <row r="729" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A729" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="B729" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="C729">
         <v>1</v>
@@ -13570,10 +13654,10 @@
     </row>
     <row r="730" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A730" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="B730" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="C730">
         <v>1</v>
@@ -13581,10 +13665,10 @@
     </row>
     <row r="731" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A731" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="B731" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="C731">
         <v>1</v>
@@ -13592,10 +13676,10 @@
     </row>
     <row r="732" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A732" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="B732" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="C732">
         <v>1</v>
@@ -13603,10 +13687,10 @@
     </row>
     <row r="733" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A733" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="B733" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="C733">
         <v>1</v>
@@ -13614,10 +13698,10 @@
     </row>
     <row r="734" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A734" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="B734" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C734">
         <v>1</v>
@@ -13625,10 +13709,10 @@
     </row>
     <row r="735" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A735" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="B735" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="C735">
         <v>1</v>
@@ -13636,10 +13720,10 @@
     </row>
     <row r="736" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A736" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="B736" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="C736">
         <v>1</v>
@@ -13647,10 +13731,10 @@
     </row>
     <row r="737" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A737" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="B737" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="C737">
         <v>1</v>
@@ -13658,10 +13742,10 @@
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A738" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="B738" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="C738">
         <v>0</v>
@@ -13669,10 +13753,10 @@
     </row>
     <row r="739" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A739" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="B739" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="C739">
         <v>1</v>
@@ -13680,10 +13764,10 @@
     </row>
     <row r="740" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A740" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="B740" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C740">
         <v>1</v>
@@ -13691,7 +13775,7 @@
     </row>
     <row r="741" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A741" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="B741" t="s">
         <v>605</v>
@@ -13700,23 +13784,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="742" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="742" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A742" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="B742" t="s">
-        <v>1397</v>
+        <v>1738</v>
       </c>
       <c r="C742">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="743" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A743" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B743" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="C743">
         <v>1</v>
@@ -13724,10 +13808,10 @@
     </row>
     <row r="744" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A744" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="B744" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="C744">
         <v>1</v>
@@ -13735,7 +13819,7 @@
     </row>
     <row r="745" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A745" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="B745" t="s">
         <v>605</v>
@@ -13746,7 +13830,7 @@
     </row>
     <row r="746" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A746" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="B746" t="s">
         <v>605</v>
@@ -13757,7 +13841,7 @@
     </row>
     <row r="747" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A747" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="B747" t="s">
         <v>605</v>
@@ -13768,10 +13852,10 @@
     </row>
     <row r="748" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A748" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="B748" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="C748">
         <v>1</v>
@@ -13779,7 +13863,7 @@
     </row>
     <row r="749" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A749" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="B749" t="s">
         <v>605</v>
@@ -13790,10 +13874,10 @@
     </row>
     <row r="750" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A750" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="B750" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="C750">
         <v>1</v>
@@ -13801,10 +13885,10 @@
     </row>
     <row r="751" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A751" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="B751" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="C751">
         <v>1</v>
@@ -13812,7 +13896,7 @@
     </row>
     <row r="752" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A752" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="B752" t="s">
         <v>605</v>
@@ -13823,10 +13907,10 @@
     </row>
     <row r="753" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A753" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="B753" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="C753">
         <v>1</v>
@@ -13834,10 +13918,10 @@
     </row>
     <row r="754" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A754" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="B754" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="C754">
         <v>1</v>
@@ -13845,10 +13929,10 @@
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A755" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="B755" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="C755">
         <v>0</v>
@@ -13856,10 +13940,10 @@
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A756" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="B756" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="C756">
         <v>0</v>
@@ -13867,10 +13951,10 @@
     </row>
     <row r="757" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A757" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="B757" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="C757">
         <v>1</v>
@@ -13878,7 +13962,7 @@
     </row>
     <row r="758" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A758" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="B758" t="s">
         <v>605</v>
@@ -13889,10 +13973,10 @@
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A759" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="B759" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="C759">
         <v>0</v>
@@ -13900,10 +13984,10 @@
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A760" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="B760" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
       <c r="C760">
         <v>0</v>
@@ -13911,7 +13995,7 @@
     </row>
     <row r="761" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A761" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="B761" t="s">
         <v>605</v>
@@ -13920,23 +14004,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="762" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="762" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A762" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="B762" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="C762">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="763" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A763" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="B763" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="C763">
         <v>1</v>
@@ -13944,10 +14028,10 @@
     </row>
     <row r="764" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A764" t="s">
-        <v>1433</v>
+        <v>1430</v>
       </c>
       <c r="B764" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
       <c r="C764">
         <v>1</v>
@@ -13955,10 +14039,10 @@
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A765" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
       <c r="B765" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="C765">
         <v>0</v>
@@ -13966,10 +14050,10 @@
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A766" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
       <c r="B766" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
       <c r="C766">
         <v>0</v>
@@ -13977,10 +14061,10 @@
     </row>
     <row r="767" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A767" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
       <c r="B767" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
       <c r="C767">
         <v>1</v>
@@ -13988,10 +14072,10 @@
     </row>
     <row r="768" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A768" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
       <c r="B768" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
       <c r="C768">
         <v>1</v>
@@ -13999,10 +14083,10 @@
     </row>
     <row r="769" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A769" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="B769" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="C769">
         <v>1</v>
@@ -14010,10 +14094,10 @@
     </row>
     <row r="770" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A770" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
       <c r="B770" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="C770">
         <v>1</v>
@@ -14021,10 +14105,10 @@
     </row>
     <row r="771" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A771" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
       <c r="B771" t="s">
-        <v>1448</v>
+        <v>1445</v>
       </c>
       <c r="C771">
         <v>1</v>
@@ -14032,10 +14116,10 @@
     </row>
     <row r="772" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A772" t="s">
-        <v>1449</v>
+        <v>1446</v>
       </c>
       <c r="B772" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
       <c r="C772">
         <v>1</v>
@@ -14043,7 +14127,7 @@
     </row>
     <row r="773" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A773" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="B773" t="s">
         <v>605</v>
@@ -14054,10 +14138,10 @@
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A774" t="s">
-        <v>1452</v>
+        <v>1449</v>
       </c>
       <c r="B774" t="s">
-        <v>1453</v>
+        <v>1450</v>
       </c>
       <c r="C774">
         <v>0</v>
@@ -14065,7 +14149,7 @@
     </row>
     <row r="775" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A775" t="s">
-        <v>1454</v>
+        <v>1451</v>
       </c>
       <c r="B775" t="s">
         <v>605</v>
@@ -14076,54 +14160,54 @@
     </row>
     <row r="776" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A776" t="s">
-        <v>1455</v>
+        <v>1452</v>
       </c>
       <c r="B776" t="s">
-        <v>1456</v>
+        <v>1453</v>
       </c>
       <c r="C776">
         <v>1</v>
       </c>
     </row>
-    <row r="777" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="777" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A777" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="B777" t="s">
-        <v>1458</v>
+        <v>1739</v>
       </c>
       <c r="C777">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A778" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
       <c r="B778" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="C778">
         <v>0</v>
       </c>
     </row>
-    <row r="779" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="779" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A779" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="B779" t="s">
-        <v>1462</v>
+        <v>1735</v>
       </c>
       <c r="C779">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A780" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="B780" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
       <c r="C780">
         <v>0</v>
@@ -14131,10 +14215,10 @@
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A781" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="B781" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
       <c r="C781">
         <v>0</v>
@@ -14142,7 +14226,7 @@
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A782" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="B782" t="s">
         <v>179</v>
@@ -14151,23 +14235,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="783" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="783" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A783" t="s">
-        <v>1468</v>
+        <v>1463</v>
       </c>
       <c r="B783" t="s">
-        <v>1469</v>
+        <v>1740</v>
       </c>
       <c r="C783">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="784" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A784" t="s">
-        <v>1470</v>
+        <v>1464</v>
       </c>
       <c r="B784" t="s">
-        <v>1471</v>
+        <v>1465</v>
       </c>
       <c r="C784">
         <v>1</v>
@@ -14175,10 +14259,10 @@
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A785" t="s">
-        <v>1472</v>
+        <v>1466</v>
       </c>
       <c r="B785" t="s">
-        <v>1473</v>
+        <v>1467</v>
       </c>
       <c r="C785">
         <v>0</v>
@@ -14186,10 +14270,10 @@
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A786" t="s">
-        <v>1474</v>
+        <v>1468</v>
       </c>
       <c r="B786" t="s">
-        <v>1475</v>
+        <v>1469</v>
       </c>
       <c r="C786">
         <v>0</v>
@@ -14197,29 +14281,29 @@
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A787" t="s">
-        <v>1476</v>
+        <v>1470</v>
       </c>
       <c r="B787" t="s">
-        <v>1477</v>
+        <v>1471</v>
       </c>
       <c r="C787">
         <v>0</v>
       </c>
     </row>
-    <row r="788" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="788" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A788" t="s">
-        <v>1478</v>
+        <v>1472</v>
       </c>
       <c r="B788" t="s">
-        <v>1479</v>
+        <v>1741</v>
       </c>
       <c r="C788">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="789" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A789" t="s">
-        <v>1480</v>
+        <v>1473</v>
       </c>
       <c r="B789" t="s">
         <v>605</v>
@@ -14230,7 +14314,7 @@
     </row>
     <row r="790" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A790" t="s">
-        <v>1481</v>
+        <v>1474</v>
       </c>
       <c r="B790" t="s">
         <v>605</v>
@@ -14241,10 +14325,10 @@
     </row>
     <row r="791" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A791" t="s">
-        <v>1482</v>
+        <v>1475</v>
       </c>
       <c r="B791" t="s">
-        <v>1483</v>
+        <v>1476</v>
       </c>
       <c r="C791">
         <v>1</v>
@@ -14252,10 +14336,10 @@
     </row>
     <row r="792" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A792" t="s">
-        <v>1484</v>
+        <v>1477</v>
       </c>
       <c r="B792" t="s">
-        <v>1485</v>
+        <v>1478</v>
       </c>
       <c r="C792">
         <v>1</v>
@@ -14263,10 +14347,10 @@
     </row>
     <row r="793" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A793" t="s">
-        <v>1486</v>
+        <v>1479</v>
       </c>
       <c r="B793" t="s">
-        <v>1487</v>
+        <v>1480</v>
       </c>
       <c r="C793">
         <v>1</v>
@@ -14274,10 +14358,10 @@
     </row>
     <row r="794" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A794" t="s">
-        <v>1488</v>
+        <v>1481</v>
       </c>
       <c r="B794" t="s">
-        <v>1489</v>
+        <v>1482</v>
       </c>
       <c r="C794">
         <v>1</v>
@@ -14285,10 +14369,10 @@
     </row>
     <row r="795" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A795" t="s">
-        <v>1490</v>
+        <v>1483</v>
       </c>
       <c r="B795" t="s">
-        <v>1491</v>
+        <v>1484</v>
       </c>
       <c r="C795">
         <v>1</v>
@@ -14296,10 +14380,10 @@
     </row>
     <row r="796" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A796" t="s">
-        <v>1492</v>
+        <v>1485</v>
       </c>
       <c r="B796" t="s">
-        <v>1493</v>
+        <v>1486</v>
       </c>
       <c r="C796">
         <v>1</v>
@@ -14307,10 +14391,10 @@
     </row>
     <row r="797" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A797" t="s">
-        <v>1494</v>
+        <v>1487</v>
       </c>
       <c r="B797" t="s">
-        <v>1495</v>
+        <v>1488</v>
       </c>
       <c r="C797">
         <v>1</v>
@@ -14318,7 +14402,7 @@
     </row>
     <row r="798" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A798" t="s">
-        <v>1496</v>
+        <v>1489</v>
       </c>
       <c r="B798" t="s">
         <v>605</v>
@@ -14329,10 +14413,10 @@
     </row>
     <row r="799" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A799" t="s">
-        <v>1497</v>
+        <v>1490</v>
       </c>
       <c r="B799" t="s">
-        <v>1498</v>
+        <v>1491</v>
       </c>
       <c r="C799">
         <v>1</v>
@@ -14340,7 +14424,7 @@
     </row>
     <row r="800" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A800" t="s">
-        <v>1499</v>
+        <v>1492</v>
       </c>
       <c r="B800" t="s">
         <v>605</v>
@@ -14351,7 +14435,7 @@
     </row>
     <row r="801" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A801" t="s">
-        <v>1500</v>
+        <v>1493</v>
       </c>
       <c r="B801" t="s">
         <v>605</v>
@@ -14362,7 +14446,7 @@
     </row>
     <row r="802" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A802" t="s">
-        <v>1501</v>
+        <v>1494</v>
       </c>
       <c r="B802" t="s">
         <v>605</v>
@@ -14373,10 +14457,10 @@
     </row>
     <row r="803" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A803" t="s">
-        <v>1502</v>
+        <v>1495</v>
       </c>
       <c r="B803" t="s">
-        <v>1503</v>
+        <v>1496</v>
       </c>
       <c r="C803">
         <v>1</v>
@@ -14384,10 +14468,10 @@
     </row>
     <row r="804" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A804" t="s">
-        <v>1504</v>
+        <v>1497</v>
       </c>
       <c r="B804" t="s">
-        <v>1505</v>
+        <v>1498</v>
       </c>
       <c r="C804">
         <v>1</v>
@@ -14395,10 +14479,10 @@
     </row>
     <row r="805" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A805" t="s">
-        <v>1506</v>
+        <v>1499</v>
       </c>
       <c r="B805" t="s">
-        <v>1507</v>
+        <v>1500</v>
       </c>
       <c r="C805">
         <v>1</v>
@@ -14406,10 +14490,10 @@
     </row>
     <row r="806" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A806" t="s">
-        <v>1508</v>
+        <v>1501</v>
       </c>
       <c r="B806" t="s">
-        <v>1509</v>
+        <v>1502</v>
       </c>
       <c r="C806">
         <v>1</v>
@@ -14417,10 +14501,10 @@
     </row>
     <row r="807" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A807" t="s">
-        <v>1510</v>
+        <v>1503</v>
       </c>
       <c r="B807" t="s">
-        <v>1511</v>
+        <v>1504</v>
       </c>
       <c r="C807">
         <v>1</v>
@@ -14428,10 +14512,10 @@
     </row>
     <row r="808" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A808" t="s">
-        <v>1512</v>
+        <v>1505</v>
       </c>
       <c r="B808" t="s">
-        <v>1513</v>
+        <v>1506</v>
       </c>
       <c r="C808">
         <v>1</v>
@@ -14439,10 +14523,10 @@
     </row>
     <row r="809" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A809" t="s">
-        <v>1514</v>
+        <v>1507</v>
       </c>
       <c r="B809" t="s">
-        <v>1515</v>
+        <v>1508</v>
       </c>
       <c r="C809">
         <v>1</v>
@@ -14450,7 +14534,7 @@
     </row>
     <row r="810" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A810" t="s">
-        <v>1516</v>
+        <v>1509</v>
       </c>
       <c r="B810" t="s">
         <v>605</v>
@@ -14461,10 +14545,10 @@
     </row>
     <row r="811" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A811" t="s">
-        <v>1517</v>
+        <v>1510</v>
       </c>
       <c r="B811" t="s">
-        <v>1518</v>
+        <v>1511</v>
       </c>
       <c r="C811">
         <v>1</v>
@@ -14472,10 +14556,10 @@
     </row>
     <row r="812" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A812" t="s">
-        <v>1519</v>
+        <v>1512</v>
       </c>
       <c r="B812" t="s">
-        <v>1520</v>
+        <v>1513</v>
       </c>
       <c r="C812">
         <v>1</v>
@@ -14483,10 +14567,10 @@
     </row>
     <row r="813" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A813" t="s">
-        <v>1521</v>
+        <v>1514</v>
       </c>
       <c r="B813" t="s">
-        <v>1522</v>
+        <v>1515</v>
       </c>
       <c r="C813">
         <v>1</v>
@@ -14494,10 +14578,10 @@
     </row>
     <row r="814" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A814" t="s">
-        <v>1523</v>
+        <v>1516</v>
       </c>
       <c r="B814" t="s">
-        <v>1524</v>
+        <v>1517</v>
       </c>
       <c r="C814">
         <v>1</v>
@@ -14505,10 +14589,10 @@
     </row>
     <row r="815" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A815" t="s">
-        <v>1525</v>
+        <v>1518</v>
       </c>
       <c r="B815" t="s">
-        <v>1526</v>
+        <v>1519</v>
       </c>
       <c r="C815">
         <v>1</v>
@@ -14516,10 +14600,10 @@
     </row>
     <row r="816" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A816" t="s">
-        <v>1527</v>
+        <v>1520</v>
       </c>
       <c r="B816" t="s">
-        <v>1528</v>
+        <v>1521</v>
       </c>
       <c r="C816">
         <v>1</v>
@@ -14527,10 +14611,10 @@
     </row>
     <row r="817" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A817" t="s">
-        <v>1529</v>
+        <v>1522</v>
       </c>
       <c r="B817" t="s">
-        <v>1530</v>
+        <v>1523</v>
       </c>
       <c r="C817">
         <v>1</v>
@@ -14538,10 +14622,10 @@
     </row>
     <row r="818" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A818" t="s">
-        <v>1531</v>
+        <v>1524</v>
       </c>
       <c r="B818" t="s">
-        <v>1532</v>
+        <v>1525</v>
       </c>
       <c r="C818">
         <v>1</v>
@@ -14549,10 +14633,10 @@
     </row>
     <row r="819" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A819" t="s">
-        <v>1533</v>
+        <v>1526</v>
       </c>
       <c r="B819" t="s">
-        <v>1534</v>
+        <v>1527</v>
       </c>
       <c r="C819">
         <v>1</v>
@@ -14560,10 +14644,10 @@
     </row>
     <row r="820" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A820" t="s">
-        <v>1535</v>
+        <v>1528</v>
       </c>
       <c r="B820" t="s">
-        <v>1536</v>
+        <v>1529</v>
       </c>
       <c r="C820">
         <v>1</v>
@@ -14571,7 +14655,7 @@
     </row>
     <row r="821" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A821" t="s">
-        <v>1537</v>
+        <v>1530</v>
       </c>
       <c r="B821" t="s">
         <v>605</v>
@@ -14582,7 +14666,7 @@
     </row>
     <row r="822" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A822" t="s">
-        <v>1538</v>
+        <v>1531</v>
       </c>
       <c r="B822" t="s">
         <v>605</v>
@@ -14593,10 +14677,10 @@
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A823" t="s">
-        <v>1539</v>
+        <v>1532</v>
       </c>
       <c r="B823" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C823">
         <v>0</v>
@@ -14604,10 +14688,10 @@
     </row>
     <row r="824" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A824" t="s">
-        <v>1540</v>
+        <v>1533</v>
       </c>
       <c r="B824" t="s">
-        <v>1541</v>
+        <v>1534</v>
       </c>
       <c r="C824">
         <v>1</v>
@@ -14615,10 +14699,10 @@
     </row>
     <row r="825" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A825" t="s">
-        <v>1542</v>
+        <v>1535</v>
       </c>
       <c r="B825" t="s">
-        <v>1543</v>
+        <v>1536</v>
       </c>
       <c r="C825">
         <v>1</v>
@@ -14626,7 +14710,7 @@
     </row>
     <row r="826" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A826" t="s">
-        <v>1544</v>
+        <v>1537</v>
       </c>
       <c r="B826" t="s">
         <v>605</v>
@@ -14637,7 +14721,7 @@
     </row>
     <row r="827" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A827" t="s">
-        <v>1545</v>
+        <v>1538</v>
       </c>
       <c r="B827" t="s">
         <v>605</v>
@@ -14648,7 +14732,7 @@
     </row>
     <row r="828" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A828" t="s">
-        <v>1546</v>
+        <v>1539</v>
       </c>
       <c r="B828" t="s">
         <v>605</v>
@@ -14659,10 +14743,10 @@
     </row>
     <row r="829" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A829" t="s">
-        <v>1547</v>
+        <v>1540</v>
       </c>
       <c r="B829" t="s">
-        <v>1548</v>
+        <v>1541</v>
       </c>
       <c r="C829">
         <v>1</v>
@@ -14670,7 +14754,7 @@
     </row>
     <row r="830" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A830" t="s">
-        <v>1549</v>
+        <v>1542</v>
       </c>
       <c r="B830" t="s">
         <v>605</v>
@@ -14681,10 +14765,10 @@
     </row>
     <row r="831" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A831" t="s">
-        <v>1550</v>
+        <v>1543</v>
       </c>
       <c r="B831" t="s">
-        <v>1551</v>
+        <v>1544</v>
       </c>
       <c r="C831">
         <v>1</v>
@@ -14692,10 +14776,10 @@
     </row>
     <row r="832" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A832" t="s">
-        <v>1552</v>
+        <v>1545</v>
       </c>
       <c r="B832" t="s">
-        <v>1553</v>
+        <v>1546</v>
       </c>
       <c r="C832">
         <v>1</v>
@@ -14703,10 +14787,10 @@
     </row>
     <row r="833" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A833" t="s">
-        <v>1554</v>
+        <v>1547</v>
       </c>
       <c r="B833" t="s">
-        <v>1555</v>
+        <v>1548</v>
       </c>
       <c r="C833">
         <v>1</v>
@@ -14714,10 +14798,10 @@
     </row>
     <row r="834" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A834" t="s">
-        <v>1556</v>
+        <v>1549</v>
       </c>
       <c r="B834" t="s">
-        <v>1557</v>
+        <v>1550</v>
       </c>
       <c r="C834">
         <v>1</v>
@@ -14725,10 +14809,10 @@
     </row>
     <row r="835" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A835" t="s">
-        <v>1558</v>
+        <v>1551</v>
       </c>
       <c r="B835" t="s">
-        <v>1559</v>
+        <v>1552</v>
       </c>
       <c r="C835">
         <v>1</v>
@@ -14736,10 +14820,10 @@
     </row>
     <row r="836" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A836" t="s">
-        <v>1560</v>
+        <v>1553</v>
       </c>
       <c r="B836" t="s">
-        <v>1561</v>
+        <v>1554</v>
       </c>
       <c r="C836">
         <v>1</v>
@@ -14747,7 +14831,7 @@
     </row>
     <row r="837" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A837" t="s">
-        <v>1562</v>
+        <v>1555</v>
       </c>
       <c r="B837" t="s">
         <v>605</v>
@@ -14758,10 +14842,10 @@
     </row>
     <row r="838" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A838" t="s">
-        <v>1563</v>
+        <v>1556</v>
       </c>
       <c r="B838" t="s">
-        <v>1564</v>
+        <v>1557</v>
       </c>
       <c r="C838">
         <v>1</v>
@@ -14769,7 +14853,7 @@
     </row>
     <row r="839" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A839" t="s">
-        <v>1565</v>
+        <v>1558</v>
       </c>
       <c r="B839" t="s">
         <v>605</v>
@@ -14780,7 +14864,7 @@
     </row>
     <row r="840" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A840" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="B840" t="s">
         <v>605</v>
@@ -14791,7 +14875,7 @@
     </row>
     <row r="841" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A841" t="s">
-        <v>1567</v>
+        <v>1560</v>
       </c>
       <c r="B841" t="s">
         <v>605</v>
@@ -14802,10 +14886,10 @@
     </row>
     <row r="842" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A842" t="s">
-        <v>1568</v>
+        <v>1561</v>
       </c>
       <c r="B842" t="s">
-        <v>1569</v>
+        <v>1562</v>
       </c>
       <c r="C842">
         <v>1</v>
@@ -14813,7 +14897,7 @@
     </row>
     <row r="843" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A843" t="s">
-        <v>1570</v>
+        <v>1563</v>
       </c>
       <c r="B843" t="s">
         <v>605</v>
@@ -14824,7 +14908,7 @@
     </row>
     <row r="844" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A844" t="s">
-        <v>1571</v>
+        <v>1564</v>
       </c>
       <c r="B844" t="s">
         <v>605</v>
@@ -14835,10 +14919,10 @@
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A845" t="s">
-        <v>1572</v>
+        <v>1565</v>
       </c>
       <c r="B845" t="s">
-        <v>1573</v>
+        <v>1566</v>
       </c>
       <c r="C845">
         <v>0</v>
@@ -14846,10 +14930,10 @@
     </row>
     <row r="846" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A846" t="s">
-        <v>1574</v>
+        <v>1567</v>
       </c>
       <c r="B846" t="s">
-        <v>1575</v>
+        <v>1568</v>
       </c>
       <c r="C846">
         <v>1</v>
@@ -14857,10 +14941,10 @@
     </row>
     <row r="847" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A847" t="s">
-        <v>1576</v>
+        <v>1569</v>
       </c>
       <c r="B847" t="s">
-        <v>1577</v>
+        <v>1570</v>
       </c>
       <c r="C847">
         <v>1</v>
@@ -14868,10 +14952,10 @@
     </row>
     <row r="848" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A848" t="s">
-        <v>1578</v>
+        <v>1571</v>
       </c>
       <c r="B848" t="s">
-        <v>1579</v>
+        <v>1572</v>
       </c>
       <c r="C848">
         <v>1</v>
@@ -14879,10 +14963,10 @@
     </row>
     <row r="849" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A849" t="s">
-        <v>1580</v>
+        <v>1573</v>
       </c>
       <c r="B849" t="s">
-        <v>1581</v>
+        <v>1574</v>
       </c>
       <c r="C849">
         <v>1</v>
@@ -14890,10 +14974,10 @@
     </row>
     <row r="850" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A850" t="s">
-        <v>1582</v>
+        <v>1575</v>
       </c>
       <c r="B850" t="s">
-        <v>1583</v>
+        <v>1576</v>
       </c>
       <c r="C850">
         <v>1</v>
@@ -14901,10 +14985,10 @@
     </row>
     <row r="851" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A851" t="s">
-        <v>1584</v>
+        <v>1577</v>
       </c>
       <c r="B851" t="s">
-        <v>1585</v>
+        <v>1578</v>
       </c>
       <c r="C851">
         <v>1</v>
@@ -14912,10 +14996,10 @@
     </row>
     <row r="852" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A852" t="s">
-        <v>1586</v>
+        <v>1579</v>
       </c>
       <c r="B852" t="s">
-        <v>1587</v>
+        <v>1580</v>
       </c>
       <c r="C852">
         <v>1</v>
@@ -14923,10 +15007,10 @@
     </row>
     <row r="853" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A853" t="s">
-        <v>1588</v>
+        <v>1581</v>
       </c>
       <c r="B853" t="s">
-        <v>1589</v>
+        <v>1582</v>
       </c>
       <c r="C853">
         <v>1</v>
@@ -14934,10 +15018,10 @@
     </row>
     <row r="854" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A854" t="s">
-        <v>1590</v>
+        <v>1583</v>
       </c>
       <c r="B854" t="s">
-        <v>1591</v>
+        <v>1584</v>
       </c>
       <c r="C854">
         <v>1</v>
@@ -14945,10 +15029,10 @@
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A855" t="s">
-        <v>1592</v>
+        <v>1585</v>
       </c>
       <c r="B855" t="s">
-        <v>1593</v>
+        <v>1586</v>
       </c>
       <c r="C855">
         <v>0</v>
@@ -14956,10 +15040,10 @@
     </row>
     <row r="856" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A856" t="s">
-        <v>1594</v>
+        <v>1587</v>
       </c>
       <c r="B856" t="s">
-        <v>1595</v>
+        <v>1588</v>
       </c>
       <c r="C856">
         <v>1</v>
@@ -14967,10 +15051,10 @@
     </row>
     <row r="857" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A857" t="s">
-        <v>1596</v>
+        <v>1589</v>
       </c>
       <c r="B857" t="s">
-        <v>1597</v>
+        <v>1590</v>
       </c>
       <c r="C857">
         <v>1</v>
@@ -14978,7 +15062,7 @@
     </row>
     <row r="858" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A858" t="s">
-        <v>1598</v>
+        <v>1591</v>
       </c>
       <c r="B858" t="s">
         <v>605</v>
@@ -14989,10 +15073,10 @@
     </row>
     <row r="859" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A859" t="s">
-        <v>1599</v>
+        <v>1592</v>
       </c>
       <c r="B859" t="s">
-        <v>1600</v>
+        <v>1593</v>
       </c>
       <c r="C859">
         <v>1</v>
@@ -15000,7 +15084,7 @@
     </row>
     <row r="860" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A860" t="s">
-        <v>1601</v>
+        <v>1594</v>
       </c>
       <c r="B860" t="s">
         <v>605</v>
@@ -15011,7 +15095,7 @@
     </row>
     <row r="861" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A861" t="s">
-        <v>1602</v>
+        <v>1595</v>
       </c>
       <c r="B861" t="s">
         <v>605</v>
@@ -15022,7 +15106,7 @@
     </row>
     <row r="862" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A862" t="s">
-        <v>1603</v>
+        <v>1596</v>
       </c>
       <c r="B862" t="s">
         <v>605</v>
@@ -15033,10 +15117,10 @@
     </row>
     <row r="863" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A863" t="s">
-        <v>1604</v>
+        <v>1597</v>
       </c>
       <c r="B863" t="s">
-        <v>1605</v>
+        <v>1598</v>
       </c>
       <c r="C863">
         <v>1</v>
@@ -15044,10 +15128,10 @@
     </row>
     <row r="864" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A864" t="s">
-        <v>1606</v>
+        <v>1599</v>
       </c>
       <c r="B864" t="s">
-        <v>1607</v>
+        <v>1600</v>
       </c>
       <c r="C864">
         <v>1</v>
@@ -15055,10 +15139,10 @@
     </row>
     <row r="865" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A865" t="s">
-        <v>1608</v>
+        <v>1601</v>
       </c>
       <c r="B865" t="s">
-        <v>1609</v>
+        <v>1602</v>
       </c>
       <c r="C865">
         <v>1</v>
@@ -15066,10 +15150,10 @@
     </row>
     <row r="866" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A866" t="s">
-        <v>1610</v>
+        <v>1603</v>
       </c>
       <c r="B866" t="s">
-        <v>1611</v>
+        <v>1604</v>
       </c>
       <c r="C866">
         <v>1</v>
@@ -15077,10 +15161,10 @@
     </row>
     <row r="867" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A867" t="s">
-        <v>1612</v>
+        <v>1605</v>
       </c>
       <c r="B867" t="s">
-        <v>1613</v>
+        <v>1606</v>
       </c>
       <c r="C867">
         <v>1</v>
@@ -15088,29 +15172,29 @@
     </row>
     <row r="868" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A868" t="s">
-        <v>1614</v>
+        <v>1607</v>
       </c>
       <c r="B868" t="s">
-        <v>1615</v>
+        <v>1608</v>
       </c>
       <c r="C868">
         <v>1</v>
       </c>
     </row>
-    <row r="869" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="869" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A869" t="s">
-        <v>1616</v>
+        <v>1609</v>
       </c>
       <c r="B869" t="s">
-        <v>1617</v>
+        <v>1610</v>
       </c>
       <c r="C869">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="870" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A870" t="s">
-        <v>1618</v>
+        <v>1611</v>
       </c>
       <c r="B870" t="s">
         <v>605</v>
@@ -15121,7 +15205,7 @@
     </row>
     <row r="871" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A871" t="s">
-        <v>1619</v>
+        <v>1612</v>
       </c>
       <c r="B871" t="s">
         <v>605</v>
@@ -15132,10 +15216,10 @@
     </row>
     <row r="872" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A872" t="s">
-        <v>1620</v>
+        <v>1613</v>
       </c>
       <c r="B872" t="s">
-        <v>1621</v>
+        <v>1614</v>
       </c>
       <c r="C872">
         <v>1</v>
@@ -15143,10 +15227,10 @@
     </row>
     <row r="873" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A873" t="s">
-        <v>1622</v>
+        <v>1615</v>
       </c>
       <c r="B873" t="s">
-        <v>1623</v>
+        <v>1616</v>
       </c>
       <c r="C873">
         <v>1</v>
@@ -15154,10 +15238,10 @@
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A874" t="s">
-        <v>1624</v>
+        <v>1617</v>
       </c>
       <c r="B874" t="s">
-        <v>1625</v>
+        <v>1618</v>
       </c>
       <c r="C874">
         <v>0</v>
@@ -15165,10 +15249,10 @@
     </row>
     <row r="875" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A875" t="s">
-        <v>1626</v>
+        <v>1619</v>
       </c>
       <c r="B875" t="s">
-        <v>1627</v>
+        <v>1620</v>
       </c>
       <c r="C875">
         <v>1</v>
@@ -15176,10 +15260,10 @@
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A876" t="s">
-        <v>1628</v>
+        <v>1621</v>
       </c>
       <c r="B876" t="s">
-        <v>1629</v>
+        <v>1622</v>
       </c>
       <c r="C876">
         <v>0</v>
@@ -15187,10 +15271,10 @@
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A877" t="s">
-        <v>1630</v>
+        <v>1623</v>
       </c>
       <c r="B877" t="s">
-        <v>1631</v>
+        <v>1624</v>
       </c>
       <c r="C877">
         <v>0</v>
@@ -15198,10 +15282,10 @@
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A878" t="s">
-        <v>1632</v>
+        <v>1625</v>
       </c>
       <c r="B878" t="s">
-        <v>1633</v>
+        <v>1626</v>
       </c>
       <c r="C878">
         <v>0</v>
@@ -15209,10 +15293,10 @@
     </row>
     <row r="879" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A879" t="s">
-        <v>1634</v>
+        <v>1627</v>
       </c>
       <c r="B879" t="s">
-        <v>1635</v>
+        <v>1628</v>
       </c>
       <c r="C879">
         <v>1</v>
@@ -15220,10 +15304,10 @@
     </row>
     <row r="880" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A880" t="s">
-        <v>1636</v>
+        <v>1629</v>
       </c>
       <c r="B880" t="s">
-        <v>1637</v>
+        <v>1630</v>
       </c>
       <c r="C880">
         <v>1</v>
@@ -15231,10 +15315,10 @@
     </row>
     <row r="881" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A881" t="s">
-        <v>1638</v>
+        <v>1631</v>
       </c>
       <c r="B881" t="s">
-        <v>1639</v>
+        <v>1632</v>
       </c>
       <c r="C881">
         <v>1</v>
@@ -15242,10 +15326,10 @@
     </row>
     <row r="882" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A882" t="s">
-        <v>1640</v>
+        <v>1633</v>
       </c>
       <c r="B882" t="s">
-        <v>1641</v>
+        <v>1634</v>
       </c>
       <c r="C882">
         <v>1</v>
@@ -15253,10 +15337,10 @@
     </row>
     <row r="883" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A883" t="s">
-        <v>1642</v>
+        <v>1635</v>
       </c>
       <c r="B883" t="s">
-        <v>1643</v>
+        <v>1636</v>
       </c>
       <c r="C883">
         <v>1</v>
@@ -15264,32 +15348,32 @@
     </row>
     <row r="884" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A884" t="s">
-        <v>1644</v>
+        <v>1637</v>
       </c>
       <c r="B884" t="s">
-        <v>1645</v>
+        <v>1638</v>
       </c>
       <c r="C884">
         <v>1</v>
       </c>
     </row>
-    <row r="885" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="885" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A885" t="s">
-        <v>1646</v>
+        <v>1639</v>
       </c>
       <c r="B885" t="s">
-        <v>1647</v>
+        <v>1742</v>
       </c>
       <c r="C885">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="886" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A886" t="s">
-        <v>1648</v>
+        <v>1640</v>
       </c>
       <c r="B886" t="s">
-        <v>1649</v>
+        <v>1641</v>
       </c>
       <c r="C886">
         <v>1</v>
@@ -15297,7 +15381,7 @@
     </row>
     <row r="887" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A887" t="s">
-        <v>1650</v>
+        <v>1642</v>
       </c>
       <c r="B887" t="s">
         <v>605</v>
@@ -15308,7 +15392,7 @@
     </row>
     <row r="888" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A888" t="s">
-        <v>1651</v>
+        <v>1643</v>
       </c>
       <c r="B888" t="s">
         <v>605</v>
@@ -15319,10 +15403,10 @@
     </row>
     <row r="889" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A889" t="s">
-        <v>1652</v>
+        <v>1644</v>
       </c>
       <c r="B889" t="s">
-        <v>1653</v>
+        <v>1645</v>
       </c>
       <c r="C889">
         <v>1</v>
@@ -15330,10 +15414,10 @@
     </row>
     <row r="890" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A890" t="s">
-        <v>1654</v>
+        <v>1646</v>
       </c>
       <c r="B890" t="s">
-        <v>1655</v>
+        <v>1647</v>
       </c>
       <c r="C890">
         <v>1</v>
@@ -15341,10 +15425,10 @@
     </row>
     <row r="891" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A891" t="s">
-        <v>1656</v>
+        <v>1648</v>
       </c>
       <c r="B891" t="s">
-        <v>1657</v>
+        <v>1649</v>
       </c>
       <c r="C891">
         <v>1</v>
@@ -15352,10 +15436,10 @@
     </row>
     <row r="892" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A892" t="s">
-        <v>1658</v>
+        <v>1650</v>
       </c>
       <c r="B892" t="s">
-        <v>1659</v>
+        <v>1651</v>
       </c>
       <c r="C892">
         <v>1</v>
@@ -15363,10 +15447,10 @@
     </row>
     <row r="893" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A893" t="s">
-        <v>1660</v>
+        <v>1652</v>
       </c>
       <c r="B893" t="s">
-        <v>1661</v>
+        <v>1653</v>
       </c>
       <c r="C893">
         <v>1</v>
@@ -15374,10 +15458,10 @@
     </row>
     <row r="894" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A894" t="s">
-        <v>1662</v>
+        <v>1654</v>
       </c>
       <c r="B894" t="s">
-        <v>1663</v>
+        <v>1655</v>
       </c>
       <c r="C894">
         <v>1</v>
@@ -15385,32 +15469,32 @@
     </row>
     <row r="895" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A895" t="s">
-        <v>1664</v>
+        <v>1656</v>
       </c>
       <c r="B895" t="s">
-        <v>1665</v>
+        <v>1657</v>
       </c>
       <c r="C895">
         <v>1</v>
       </c>
     </row>
-    <row r="896" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="896" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A896" t="s">
-        <v>1666</v>
+        <v>1658</v>
       </c>
       <c r="B896" t="s">
-        <v>1397</v>
+        <v>1743</v>
       </c>
       <c r="C896">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="897" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A897" t="s">
-        <v>1667</v>
+        <v>1659</v>
       </c>
       <c r="B897" t="s">
-        <v>1668</v>
+        <v>1660</v>
       </c>
       <c r="C897">
         <v>1</v>
@@ -15418,10 +15502,10 @@
     </row>
     <row r="898" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A898" t="s">
-        <v>1669</v>
+        <v>1661</v>
       </c>
       <c r="B898" t="s">
-        <v>1670</v>
+        <v>1662</v>
       </c>
       <c r="C898">
         <v>1</v>
@@ -15429,10 +15513,10 @@
     </row>
     <row r="899" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A899" t="s">
-        <v>1671</v>
+        <v>1663</v>
       </c>
       <c r="B899" t="s">
-        <v>1672</v>
+        <v>1664</v>
       </c>
       <c r="C899">
         <v>1</v>
@@ -15440,7 +15524,7 @@
     </row>
     <row r="900" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A900" t="s">
-        <v>1673</v>
+        <v>1665</v>
       </c>
       <c r="B900" t="s">
         <v>605</v>
@@ -15451,10 +15535,10 @@
     </row>
     <row r="901" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A901" t="s">
-        <v>1674</v>
+        <v>1666</v>
       </c>
       <c r="B901" t="s">
-        <v>1675</v>
+        <v>1667</v>
       </c>
       <c r="C901">
         <v>1</v>
@@ -15462,10 +15546,10 @@
     </row>
     <row r="902" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A902" t="s">
-        <v>1676</v>
+        <v>1668</v>
       </c>
       <c r="B902" t="s">
-        <v>1677</v>
+        <v>1669</v>
       </c>
       <c r="C902">
         <v>1</v>
@@ -15473,10 +15557,10 @@
     </row>
     <row r="903" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A903" t="s">
-        <v>1678</v>
+        <v>1670</v>
       </c>
       <c r="B903" t="s">
-        <v>1679</v>
+        <v>1671</v>
       </c>
       <c r="C903">
         <v>1</v>
@@ -15484,10 +15568,10 @@
     </row>
     <row r="904" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A904" t="s">
-        <v>1680</v>
+        <v>1672</v>
       </c>
       <c r="B904" t="s">
-        <v>1681</v>
+        <v>1673</v>
       </c>
       <c r="C904">
         <v>1</v>
@@ -15495,10 +15579,10 @@
     </row>
     <row r="905" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A905" t="s">
-        <v>1682</v>
+        <v>1674</v>
       </c>
       <c r="B905" t="s">
-        <v>1683</v>
+        <v>1675</v>
       </c>
       <c r="C905">
         <v>1</v>
@@ -15506,43 +15590,43 @@
     </row>
     <row r="906" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A906" t="s">
-        <v>1684</v>
+        <v>1676</v>
       </c>
       <c r="B906" t="s">
-        <v>1685</v>
+        <v>1677</v>
       </c>
       <c r="C906">
         <v>1</v>
       </c>
     </row>
-    <row r="907" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="907" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A907" t="s">
-        <v>1686</v>
+        <v>1678</v>
       </c>
       <c r="B907" t="s">
-        <v>1687</v>
+        <v>1744</v>
       </c>
       <c r="C907">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="908" spans="1:3" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A908" t="s">
-        <v>1688</v>
+        <v>1679</v>
       </c>
       <c r="B908" t="s">
-        <v>1689</v>
+        <v>1680</v>
       </c>
       <c r="C908">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="909" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A909" t="s">
-        <v>1690</v>
+        <v>1681</v>
       </c>
       <c r="B909" t="s">
-        <v>1691</v>
+        <v>1682</v>
       </c>
       <c r="C909">
         <v>1</v>
@@ -15550,10 +15634,10 @@
     </row>
     <row r="910" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A910" t="s">
-        <v>1692</v>
+        <v>1683</v>
       </c>
       <c r="B910" t="s">
-        <v>1693</v>
+        <v>1684</v>
       </c>
       <c r="C910">
         <v>1</v>
@@ -15561,7 +15645,7 @@
     </row>
     <row r="911" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A911" t="s">
-        <v>1694</v>
+        <v>1685</v>
       </c>
       <c r="B911" t="s">
         <v>605</v>
@@ -15572,10 +15656,10 @@
     </row>
     <row r="912" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A912" t="s">
-        <v>1695</v>
+        <v>1686</v>
       </c>
       <c r="B912" t="s">
-        <v>1696</v>
+        <v>1687</v>
       </c>
       <c r="C912">
         <v>1</v>
@@ -15583,7 +15667,7 @@
     </row>
     <row r="913" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A913" t="s">
-        <v>1697</v>
+        <v>1688</v>
       </c>
       <c r="B913" t="s">
         <v>605</v>
@@ -15594,10 +15678,10 @@
     </row>
     <row r="914" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A914" t="s">
-        <v>1698</v>
+        <v>1689</v>
       </c>
       <c r="B914" t="s">
-        <v>1699</v>
+        <v>1690</v>
       </c>
       <c r="C914">
         <v>1</v>
@@ -15605,7 +15689,7 @@
     </row>
     <row r="915" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A915" t="s">
-        <v>1700</v>
+        <v>1691</v>
       </c>
       <c r="B915" t="s">
         <v>605</v>
@@ -15616,10 +15700,10 @@
     </row>
     <row r="916" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A916" t="s">
-        <v>1701</v>
+        <v>1692</v>
       </c>
       <c r="B916" t="s">
-        <v>1702</v>
+        <v>1693</v>
       </c>
       <c r="C916">
         <v>1</v>
@@ -15627,10 +15711,10 @@
     </row>
     <row r="917" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A917" t="s">
-        <v>1703</v>
+        <v>1694</v>
       </c>
       <c r="B917" t="s">
-        <v>1704</v>
+        <v>1695</v>
       </c>
       <c r="C917">
         <v>1</v>
@@ -15638,7 +15722,7 @@
     </row>
     <row r="918" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A918" t="s">
-        <v>1705</v>
+        <v>1696</v>
       </c>
       <c r="B918" t="s">
         <v>605</v>
@@ -15649,10 +15733,10 @@
     </row>
     <row r="919" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A919" t="s">
-        <v>1706</v>
+        <v>1697</v>
       </c>
       <c r="B919" t="s">
-        <v>1707</v>
+        <v>1698</v>
       </c>
       <c r="C919">
         <v>1</v>
@@ -15660,10 +15744,10 @@
     </row>
     <row r="920" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A920" t="s">
-        <v>1708</v>
+        <v>1699</v>
       </c>
       <c r="B920" t="s">
-        <v>1709</v>
+        <v>1700</v>
       </c>
       <c r="C920">
         <v>1</v>
@@ -15671,7 +15755,7 @@
     </row>
     <row r="921" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A921" t="s">
-        <v>1710</v>
+        <v>1701</v>
       </c>
       <c r="B921" t="s">
         <v>605</v>
@@ -15682,7 +15766,7 @@
     </row>
     <row r="922" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A922" t="s">
-        <v>1711</v>
+        <v>1702</v>
       </c>
       <c r="B922" t="s">
         <v>605</v>
@@ -15693,7 +15777,7 @@
     </row>
     <row r="923" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A923" t="s">
-        <v>1712</v>
+        <v>1703</v>
       </c>
       <c r="B923" t="s">
         <v>605</v>
@@ -15704,7 +15788,7 @@
     </row>
     <row r="924" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A924" t="s">
-        <v>1713</v>
+        <v>1704</v>
       </c>
       <c r="B924" t="s">
         <v>605</v>
@@ -15715,10 +15799,10 @@
     </row>
     <row r="925" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A925" t="s">
-        <v>1714</v>
+        <v>1705</v>
       </c>
       <c r="B925" t="s">
-        <v>1715</v>
+        <v>1706</v>
       </c>
       <c r="C925">
         <v>1</v>
@@ -15726,7 +15810,7 @@
     </row>
     <row r="926" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A926" t="s">
-        <v>1716</v>
+        <v>1707</v>
       </c>
       <c r="B926" t="s">
         <v>605</v>
@@ -15737,10 +15821,10 @@
     </row>
     <row r="927" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A927" t="s">
-        <v>1717</v>
+        <v>1708</v>
       </c>
       <c r="B927" t="s">
-        <v>1718</v>
+        <v>1709</v>
       </c>
       <c r="C927">
         <v>1</v>
@@ -15748,17 +15832,171 @@
     </row>
     <row r="928" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
       <c r="A928" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B928" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C928">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="929" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A929" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B929" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C929">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A930" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B930" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C930">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A931" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B931" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C931">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A932" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B932" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C932">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="933" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A933" t="s">
         <v>1719</v>
       </c>
-      <c r="B928" t="s">
+      <c r="B933" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C933">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A934" t="s">
         <v>1720</v>
       </c>
-      <c r="C928">
+      <c r="B934" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C934">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="935" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A935" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B935" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C935">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="936" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A936" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B936" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C936">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="937" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A937" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B937" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C937">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="938" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A938" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B938" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C938">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="939" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A939" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B939" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C939">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="940" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A940" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B940" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C940">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="941" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A941" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B941" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C941">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="942" spans="1:3" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A942" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B942" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C942">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C928" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="C1:C942" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="0"/>

</xml_diff>

<commit_message>
update rules to v22
</commit_message>
<xml_diff>
--- a/pkg-info.xlsx
+++ b/pkg-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Documents\Source Codes\gkd-rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B952F11-6E50-49E6-96B0-67B8DA653315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD444FD3-0BF8-4898-B92F-DF7B7E490706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="1594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="1868">
   <si>
     <t>package_name</t>
   </si>
@@ -4802,6 +4802,833 @@
   </si>
   <si>
     <t>大麦</t>
+  </si>
+  <si>
+    <t>com.mfashiongallery.emag</t>
+  </si>
+  <si>
+    <t>小米画报</t>
+  </si>
+  <si>
+    <t>li.songe.gkd</t>
+  </si>
+  <si>
+    <t>GKD</t>
+  </si>
+  <si>
+    <t>com.tencent.wetype</t>
+  </si>
+  <si>
+    <t>微信输入法</t>
+  </si>
+  <si>
+    <t>com.github.android</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>org.telegram.messenger</t>
+  </si>
+  <si>
+    <t>com.aistra.hail</t>
+  </si>
+  <si>
+    <t>Hail</t>
+  </si>
+  <si>
+    <t>com.perol.play.pixez</t>
+  </si>
+  <si>
+    <t>PixEz Flutter</t>
+  </si>
+  <si>
+    <t>ru.zdevs.zarchiver</t>
+  </si>
+  <si>
+    <t>Zarchiver</t>
+  </si>
+  <si>
+    <t>ru.zdevs.zarchiver.pro</t>
+  </si>
+  <si>
+    <t>me.zhanghai.android.files</t>
+  </si>
+  <si>
+    <t>Material Files</t>
+  </si>
+  <si>
+    <t>com.ktls.fileinfo</t>
+  </si>
+  <si>
+    <t>存储空间清理</t>
+  </si>
+  <si>
+    <t>idm.internet.download.manager</t>
+  </si>
+  <si>
+    <t>1DM</t>
+  </si>
+  <si>
+    <t>idm.internet.download.manager.plus</t>
+  </si>
+  <si>
+    <t>1DM+</t>
+  </si>
+  <si>
+    <t>org.adblockplus.adblockplussbrowser</t>
+  </si>
+  <si>
+    <t>ABP for Samsung Internet</t>
+  </si>
+  <si>
+    <t>com.pittvandewitt.wavelet</t>
+  </si>
+  <si>
+    <t>Wavelet: headphone specific EQ</t>
+  </si>
+  <si>
+    <t>com.miui.weather2</t>
+  </si>
+  <si>
+    <t>小米天气</t>
+  </si>
+  <si>
+    <t>com.heytap.browser</t>
+  </si>
+  <si>
+    <t>Internet Browser</t>
+  </si>
+  <si>
+    <t>com.heytap.themestore</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>com.guozhigq.pilipala</t>
+  </si>
+  <si>
+    <t>PiliPala</t>
+  </si>
+  <si>
+    <t>com.salt.music</t>
+  </si>
+  <si>
+    <t>Salt Player</t>
+  </si>
+  <si>
+    <t>com.v2ray.ang</t>
+  </si>
+  <si>
+    <t>v2rayNG</t>
+  </si>
+  <si>
+    <t>com.xiaoyv.bangumi</t>
+  </si>
+  <si>
+    <t>Bangumi for Android</t>
+  </si>
+  <si>
+    <t>com.looker.droidify</t>
+  </si>
+  <si>
+    <t>Droid-ify</t>
+  </si>
+  <si>
+    <t>app.eleven.com.fastfiletransfer</t>
+  </si>
+  <si>
+    <t>文件闪传</t>
+  </si>
+  <si>
+    <t>com.idaodan.clean.master</t>
+  </si>
+  <si>
+    <t>雪豹速清</t>
+  </si>
+  <si>
+    <t>app.rikka.savecopy</t>
+  </si>
+  <si>
+    <t>Save Copy</t>
+  </si>
+  <si>
+    <t>com.dv.adm</t>
+  </si>
+  <si>
+    <t>Advanced Download Manager</t>
+  </si>
+  <si>
+    <t>org.koitharu.kotatsu</t>
+  </si>
+  <si>
+    <t>Kotatsu</t>
+  </si>
+  <si>
+    <t>me.ash.reader</t>
+  </si>
+  <si>
+    <t>Read You</t>
+  </si>
+  <si>
+    <t>dev.anilbeesetti.nextplayer</t>
+  </si>
+  <si>
+    <t>Next Player</t>
+  </si>
+  <si>
+    <t>org.kde.kdeconnect_tp</t>
+  </si>
+  <si>
+    <t>KDE Connect</t>
+  </si>
+  <si>
+    <t>one.yufz.hmspush</t>
+  </si>
+  <si>
+    <t>未知</t>
+  </si>
+  <si>
+    <t>io.github.huskydg.magisk</t>
+  </si>
+  <si>
+    <t>xzr.konabess</t>
+  </si>
+  <si>
+    <t>org.lsposed.manager</t>
+  </si>
+  <si>
+    <t>LSPosed</t>
+  </si>
+  <si>
+    <t>com.microsoft.office.officehub</t>
+  </si>
+  <si>
+    <t>Office Mobile for Office 365</t>
+  </si>
+  <si>
+    <t>io.github.qauxv</t>
+  </si>
+  <si>
+    <t>com.rezvorck.tiktokplugin</t>
+  </si>
+  <si>
+    <t>com.github.tianma8023.xposed.smscode</t>
+  </si>
+  <si>
+    <t>Han.GJZS</t>
+  </si>
+  <si>
+    <t>com.viewblocker.jrsen</t>
+  </si>
+  <si>
+    <t>com.tsng.hidemyapplist</t>
+  </si>
+  <si>
+    <t>com.miui.calculator</t>
+  </si>
+  <si>
+    <t>计算器</t>
+  </si>
+  <si>
+    <t>com.android.email</t>
+  </si>
+  <si>
+    <t>邮件</t>
+  </si>
+  <si>
+    <t>com.miui.screenrecorder</t>
+  </si>
+  <si>
+    <t>屏幕录制</t>
+  </si>
+  <si>
+    <t>com.android.deskclock</t>
+  </si>
+  <si>
+    <t>时钟</t>
+  </si>
+  <si>
+    <t>com.miui.newmidrive</t>
+  </si>
+  <si>
+    <t>小米云盘</t>
+  </si>
+  <si>
+    <t>cn.wps.moffice_eng.xiaomi.lite</t>
+  </si>
+  <si>
+    <t>小米文档查看器（WPS定制）</t>
+  </si>
+  <si>
+    <t>com.miui.mediaeditor</t>
+  </si>
+  <si>
+    <t>媒体编辑器</t>
+  </si>
+  <si>
+    <t>com.samsung.android.app.cameraassistant</t>
+  </si>
+  <si>
+    <t>Camera Assistant</t>
+  </si>
+  <si>
+    <t>com.samsung.android.app.galaxyraw</t>
+  </si>
+  <si>
+    <t>Expert RAW</t>
+  </si>
+  <si>
+    <t>com.samsung.android.appbooster</t>
+  </si>
+  <si>
+    <t>Galaxy App Booster</t>
+  </si>
+  <si>
+    <t>com.android.samsung.utilityapp</t>
+  </si>
+  <si>
+    <t>Good Guardians</t>
+  </si>
+  <si>
+    <t>com.samsung.android.goodlock</t>
+  </si>
+  <si>
+    <t>Good Lock</t>
+  </si>
+  <si>
+    <t>com.samsung.android.thermalguardian</t>
+  </si>
+  <si>
+    <t>Thermal Guardian</t>
+  </si>
+  <si>
+    <t>com.samsung.android.calendar</t>
+  </si>
+  <si>
+    <t>Samsung Calendar</t>
+  </si>
+  <si>
+    <t>com.samsung.android.app.notes</t>
+  </si>
+  <si>
+    <t>Samsung Notes</t>
+  </si>
+  <si>
+    <t>com.jv.samsungeshop</t>
+  </si>
+  <si>
+    <t>三星商城</t>
+  </si>
+  <si>
+    <t>com.samsung.android.app.sreminder</t>
+  </si>
+  <si>
+    <t>三星生活助手</t>
+  </si>
+  <si>
+    <t>com.samsung.android.app.watchmanager</t>
+  </si>
+  <si>
+    <t>三星智能穿戴</t>
+  </si>
+  <si>
+    <t>com.samsung.android.app.reminder</t>
+  </si>
+  <si>
+    <t>Reminder</t>
+  </si>
+  <si>
+    <t>com.adguard.android.contentblocker</t>
+  </si>
+  <si>
+    <t>AdGuard: Content Blocker</t>
+  </si>
+  <si>
+    <t>com.mmbox.xbrowser</t>
+  </si>
+  <si>
+    <t>X浏览器</t>
+  </si>
+  <si>
+    <t>com.mmbox.xbrowser.pro</t>
+  </si>
+  <si>
+    <t>com.mycompany.app.soulbrowser</t>
+  </si>
+  <si>
+    <t>Soul Browser</t>
+  </si>
+  <si>
+    <t>com.miui.notes</t>
+  </si>
+  <si>
+    <t>小米笔记</t>
+  </si>
+  <si>
+    <t>com.miui.cleanmaster</t>
+  </si>
+  <si>
+    <t>垃圾清理</t>
+  </si>
+  <si>
+    <t>com.miui.compass</t>
+  </si>
+  <si>
+    <t>指南针</t>
+  </si>
+  <si>
+    <t>mark.via</t>
+  </si>
+  <si>
+    <t>Via</t>
+  </si>
+  <si>
+    <t>mark.via.gp</t>
+  </si>
+  <si>
+    <t>Via Browser</t>
+  </si>
+  <si>
+    <t>com.bug.hookvip</t>
+  </si>
+  <si>
+    <t>HookVIP</t>
+  </si>
+  <si>
+    <t>one.yufz.onebox</t>
+  </si>
+  <si>
+    <t>com.sec.android.app.voicenote</t>
+  </si>
+  <si>
+    <t>Samsung Voice Recorder</t>
+  </si>
+  <si>
+    <t>com.xy.td</t>
+  </si>
+  <si>
+    <t>com.futuremark.dmandroid.application</t>
+  </si>
+  <si>
+    <t>3DMark</t>
+  </si>
+  <si>
+    <t>com.sec.android.app.clockpackage</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>com.xuncorp.qinalt.music</t>
+  </si>
+  <si>
+    <t>xyz.adproqwq.GKDTool</t>
+  </si>
+  <si>
+    <t>xyz.nextalone.nagram</t>
+  </si>
+  <si>
+    <t>com.openai.chatgpt</t>
+  </si>
+  <si>
+    <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>org.telegram.group</t>
+  </si>
+  <si>
+    <t>Turrit</t>
+  </si>
+  <si>
+    <t>com.android.chrome</t>
+  </si>
+  <si>
+    <t>谷歌浏览器Google Chrome</t>
+  </si>
+  <si>
+    <t>com.magicalstory.videos</t>
+  </si>
+  <si>
+    <t>com.magicalstory.installer</t>
+  </si>
+  <si>
+    <t>com.mxtech.videoplayer.pro</t>
+  </si>
+  <si>
+    <t>MX Player Pro</t>
+  </si>
+  <si>
+    <t>com.github.kr328.clash</t>
+  </si>
+  <si>
+    <t>com.x8bit.bitwarden</t>
+  </si>
+  <si>
+    <t>Bitwarden Password Manager</t>
+  </si>
+  <si>
+    <t>org.localsend.localsend_app</t>
+  </si>
+  <si>
+    <t>LocalSend: FOSS Airdrop</t>
+  </si>
+  <si>
+    <t>moe.shizuku.privileged.api</t>
+  </si>
+  <si>
+    <t>Shizuku</t>
+  </si>
+  <si>
+    <t>com.ktls.automation</t>
+  </si>
+  <si>
+    <t>com.deepl.mobiletranslator</t>
+  </si>
+  <si>
+    <t>DeepL</t>
+  </si>
+  <si>
+    <t>com.accessibilitymanager</t>
+  </si>
+  <si>
+    <t>me.tasy5kg.cutegif</t>
+  </si>
+  <si>
+    <t>com.absinthe.libchecker</t>
+  </si>
+  <si>
+    <t>LibChecker</t>
+  </si>
+  <si>
+    <t>com.github.metacubex.clash.meta</t>
+  </si>
+  <si>
+    <t>ClashMetaForAndroid</t>
+  </si>
+  <si>
+    <t>app.mihon</t>
+  </si>
+  <si>
+    <t>com.rosan.installer.x</t>
+  </si>
+  <si>
+    <t>com.rosan.dhizuku</t>
+  </si>
+  <si>
+    <t>com.rosan.accounts</t>
+  </si>
+  <si>
+    <t>com.assistant.ongoingclear</t>
+  </si>
+  <si>
+    <t>com.huanchengfly.tieba.post</t>
+  </si>
+  <si>
+    <t>com.example.c001apk</t>
+  </si>
+  <si>
+    <t>moe.nb4a</t>
+  </si>
+  <si>
+    <t>NekoBox for Android</t>
+  </si>
+  <si>
+    <t>com.funny.translation</t>
+  </si>
+  <si>
+    <t>com.samsung.agc.gcam84</t>
+  </si>
+  <si>
+    <t>com.wsw.cospa</t>
+  </si>
+  <si>
+    <t>io.github.jd1378.otphelper</t>
+  </si>
+  <si>
+    <t>Copy SMS Code</t>
+  </si>
+  <si>
+    <t>com.valvesoftware.android.steam.community</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>io.legado.app.release</t>
+  </si>
+  <si>
+    <t>com.getsurfboard</t>
+  </si>
+  <si>
+    <t>Surfboard</t>
+  </si>
+  <si>
+    <t>com.heyanle.easybangumi4</t>
+  </si>
+  <si>
+    <t>com.perol.pixez</t>
+  </si>
+  <si>
+    <t>com.github.wgh136.pica_comic</t>
+  </si>
+  <si>
+    <t>com.yenaly.han1meviewer</t>
+  </si>
+  <si>
+    <t>com.xjcheng.musictageditor</t>
+  </si>
+  <si>
+    <t>com.lalilu.lmusic</t>
+  </si>
+  <si>
+    <t>com.mxtech.videoplayer</t>
+  </si>
+  <si>
+    <t>com.tencent.southpole.appstore</t>
+  </si>
+  <si>
+    <t>org.mozilla.firefox</t>
+  </si>
+  <si>
+    <t>火狐浏览器</t>
+  </si>
+  <si>
+    <t>com.mixplorer</t>
+  </si>
+  <si>
+    <t>MiXplorer</t>
+  </si>
+  <si>
+    <t>com.xjs.ehviewer</t>
+  </si>
+  <si>
+    <t>rikka.appops</t>
+  </si>
+  <si>
+    <t>App Ops</t>
+  </si>
+  <si>
+    <t>com.vrem.wifianalyzer</t>
+  </si>
+  <si>
+    <t>WiFi Analyzer</t>
+  </si>
+  <si>
+    <t>remix.myplayer</t>
+  </si>
+  <si>
+    <t>APlayer</t>
+  </si>
+  <si>
+    <t>com.arn.scrobble</t>
+  </si>
+  <si>
+    <t>Pano Scrobbler for LastFM</t>
+  </si>
+  <si>
+    <t>org.videolan.vlc</t>
+  </si>
+  <si>
+    <t>VLC for Android</t>
+  </si>
+  <si>
+    <t>org.geogebra.android.calculator.suite</t>
+  </si>
+  <si>
+    <t>GeoGebra Calculator Suite</t>
+  </si>
+  <si>
+    <t>com.azure.authenticator</t>
+  </si>
+  <si>
+    <t>Authenticator</t>
+  </si>
+  <si>
+    <t>com.microsoft.office.officehubrow</t>
+  </si>
+  <si>
+    <t>Microsoft 365 (Office)</t>
+  </si>
+  <si>
+    <t>com.microsoft.office.outlook</t>
+  </si>
+  <si>
+    <t>Outlook</t>
+  </si>
+  <si>
+    <t>com.microsoft.office.onenote</t>
+  </si>
+  <si>
+    <t>OneNote</t>
+  </si>
+  <si>
+    <t>com.sonkins.tguitar</t>
+  </si>
+  <si>
+    <t>Guitar Tuner</t>
+  </si>
+  <si>
+    <t>com.eumlab.android.prometronome</t>
+  </si>
+  <si>
+    <t>Pro Metronome 专业节拍器</t>
+  </si>
+  <si>
+    <t>com.Wecrane.Scar.pubg</t>
+  </si>
+  <si>
+    <t>me.bmax.apatch</t>
+  </si>
+  <si>
+    <t>com.tubevpn.client</t>
+  </si>
+  <si>
+    <t>github.tornaco.android.thanos.pro</t>
+  </si>
+  <si>
+    <t>Thanox Pro</t>
+  </si>
+  <si>
+    <t>com.omarea.vtools</t>
+  </si>
+  <si>
+    <t>com.litebyte.samhelper</t>
+  </si>
+  <si>
+    <t>com.nurke.perfectone</t>
+  </si>
+  <si>
+    <t>qlenlen.OneDesign</t>
+  </si>
+  <si>
+    <t>icu.nullptr.nativetest</t>
+  </si>
+  <si>
+    <t>io.github.vvb2060.mahoshojo</t>
+  </si>
+  <si>
+    <t>com.samsung.android.memoryguardian</t>
+  </si>
+  <si>
+    <t>Memory Guardian</t>
+  </si>
+  <si>
+    <t>com.music.khkj</t>
+  </si>
+  <si>
+    <t>Hook.JiuWu.Xp</t>
+  </si>
+  <si>
+    <t>me.weishu.kernelsu</t>
+  </si>
+  <si>
+    <t>com.franco.kernel</t>
+  </si>
+  <si>
+    <t>Franco Kernel Manager</t>
+  </si>
+  <si>
+    <t>com.molink.john.hummingbird</t>
+  </si>
+  <si>
+    <t>bebird</t>
+  </si>
+  <si>
+    <t>com.samsung.android.themedesigner</t>
+  </si>
+  <si>
+    <t>Theme Park</t>
+  </si>
+  <si>
+    <t>com.samsung.android.game.gamehome</t>
+  </si>
+  <si>
+    <t>Gaming Hub</t>
+  </si>
+  <si>
+    <t>com.tencent.tmgp.sgame</t>
+  </si>
+  <si>
+    <t>王者荣耀</t>
+  </si>
+  <si>
+    <t>com.yangyanghuzhou.heijuan</t>
+  </si>
+  <si>
+    <t>com.sec.android.app.sbrowser</t>
+  </si>
+  <si>
+    <t>Samsung Internet Browser</t>
+  </si>
+  <si>
+    <t>com.samsung.android.game.gamelab</t>
+  </si>
+  <si>
+    <t>Game Plugins</t>
+  </si>
+  <si>
+    <t>com.Twilight.tools</t>
+  </si>
+  <si>
+    <t>com.miui.securitymanager</t>
+  </si>
+  <si>
+    <t>com.android.settings</t>
+  </si>
+  <si>
+    <t>com.miui.creation</t>
+  </si>
+  <si>
+    <t>com.yozo.office</t>
+  </si>
+  <si>
+    <t>永中Office</t>
+  </si>
+  <si>
+    <t>com.xiaomi.wpslauncher</t>
+  </si>
+  <si>
+    <t>com.sevtinge.hyperceiler</t>
+  </si>
+  <si>
+    <t>com.dna.tools</t>
+  </si>
+  <si>
+    <t>flar2.devcheck</t>
+  </si>
+  <si>
+    <t>DevCheck Device &amp;amp; System Info</t>
+  </si>
+  <si>
+    <t>com.gstarmc.android</t>
+  </si>
+  <si>
+    <t>CAD看图王</t>
+  </si>
+  <si>
+    <t>com.miui.thirdappassistant</t>
+  </si>
+  <si>
+    <t>安全管家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米创作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三方应用异常分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无障碍管理器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5150,10 +5977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C807"/>
+  <dimension ref="A1:C973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A793" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A811" sqref="A811"/>
+    <sheetView tabSelected="1" topLeftCell="A843" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C844" sqref="C844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14040,6 +14867,1832 @@
         <v>1</v>
       </c>
     </row>
+    <row r="808" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A808" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B808" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C808">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A809" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B809" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C809">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A810" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B810" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C810">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A811" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B811" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C811">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A812" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B812" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C812">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="813" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A813" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B813" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C813">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A814" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B814" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C814">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A815" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B815" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C815">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A816" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B816" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C816">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A817" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B817" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C817">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A818" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B818" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C818">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A819" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C819">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A820" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B820" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C820">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A821" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B821" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C821">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A822" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B822" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C822">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A823" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B823" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C823">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A824" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B824" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C824">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A825" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B825" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C825">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A826" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B826" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C826">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A827" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B827" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C827">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="828" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A828" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B828" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C828">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A829" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B829" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C829">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A830" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B830" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C830">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A831" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B831" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C831">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A832" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B832" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C832">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A833" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B833" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C833">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A834" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B834" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C834">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="835" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A835" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B835" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C835">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="836" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A836" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B836" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C836">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="837" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A837" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B837" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C837">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="838" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A838" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B838" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C838">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="839" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A839" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B839" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C839">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="840" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A840" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B840" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C840">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A841" t="s">
+        <v>1657</v>
+      </c>
+      <c r="B841" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C841">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="842" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A842" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B842" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C842">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="843" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A843" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B843" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C843">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="844" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A844" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B844" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C844">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="845" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A845" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B845" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C845">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="846" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A846" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B846" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C846">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="847" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A847" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B847" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C847">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="848" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A848" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B848" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C848">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="849" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A849" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B849" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C849">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="850" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A850" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B850" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C850">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="851" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A851" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B851" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C851">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="852" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A852" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B852" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C852">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="853" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A853" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B853" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C853">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="854" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A854" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B854" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C854">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="855" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A855" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B855" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C855">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="856" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A856" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B856" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C856">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="857" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A857" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B857" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C857">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="858" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A858" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B858" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C858">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A859" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B859" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C859">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A860" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B860" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C860">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A861" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B861" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C861">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A862" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B862" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C862">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A863" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B863" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C863">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="864" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A864" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B864" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C864">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A865" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B865" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C865">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A866" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B866" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C866">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A867" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B867" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C867">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A868" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B868" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C868">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A869" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B869" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C869">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="870" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A870" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B870" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C870">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="871" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A871" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B871" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C871">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="872" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A872" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B872" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C872">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="873" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A873" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B873" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C873">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="874" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A874" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B874" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C874">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="875" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A875" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B875" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C875">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="876" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A876" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B876" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C876">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="877" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A877" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B877" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C877">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="878" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A878" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B878" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C878">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="879" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A879" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B879" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C879">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="880" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A880" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B880" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C880">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="881" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A881" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B881" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C881">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="882" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A882" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B882" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C882">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="883" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A883" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B883" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C883">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="884" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A884" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B884" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C884">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="885" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A885" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C885">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A886" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C886">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="887" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A887" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C887">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="888" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A888" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C888">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="889" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A889" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C889">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="890" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A890" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C890">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="891" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A891" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B891" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C891">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="892" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A892" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B892" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C892">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="893" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A893" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B893" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C893">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="894" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A894" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B894" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C894">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A895" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B895" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C895">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="896" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A896" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C896">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="897" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A897" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B897" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C897">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A898" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B898" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C898">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="899" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A899" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B899" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C899">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A900" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B900" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C900">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A901" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B901" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C901">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="902" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A902" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B902" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C902">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="903" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A903" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B903" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C903">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A904" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B904" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C904">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="905" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A905" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B905" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C905">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A906" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B906" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C906">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="907" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A907" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B907" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C907">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A908" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B908" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C908">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="909" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A909" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B909" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C909">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="910" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A910" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B910" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C910">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="911" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A911" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B911" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C911">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="912" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A912" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B912" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C912">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="913" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A913" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B913" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C913">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="914" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A914" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B914" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C914">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="915" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A915" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B915" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C915">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="916" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A916" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B916" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C916">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="917" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A917" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B917" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C917">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="918" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A918" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B918" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C918">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="919" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A919" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B919" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C919">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="920" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A920" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B920" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C920">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="921" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A921" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B921" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C921">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="922" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A922" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B922" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C922">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="923" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A923" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B923" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C923">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="924" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A924" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B924" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C924">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="925" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A925" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B925" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C925">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="926" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A926" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B926" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C926">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="927" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A927" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B927" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C927">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="928" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A928" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B928" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C928">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="929" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A929" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B929" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C929">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A930" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B930" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C930">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A931" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B931" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C931">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A932" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B932" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C932">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="933" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A933" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B933" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C933">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A934" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B934" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C934">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="935" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A935" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B935" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C935">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="936" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A936" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B936" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C936">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="937" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A937" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B937" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C937">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="938" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A938" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B938" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C938">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="939" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A939" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B939" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C939">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="940" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A940" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B940" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C940">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="941" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A941" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B941" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C941">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="942" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A942" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B942" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C942">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="943" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A943" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B943" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C943">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="944" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A944" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B944" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C944">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="945" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A945" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B945" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C945">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="946" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A946" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B946" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C946">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="947" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A947" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B947" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C947">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="948" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A948" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B948" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C948">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="949" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A949" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B949" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C949">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="950" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A950" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B950" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C950">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="951" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A951" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B951" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C951">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="952" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A952" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B952" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C952">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="953" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A953" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B953" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C953">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="954" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A954" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B954" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C954">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="955" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A955" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B955" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C955">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="956" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A956" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C956">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="957" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A957" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C957">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="958" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A958" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C958">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="959" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A959" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C959">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="960" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A960" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B960" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C960">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="961" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A961" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C961">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="962" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A962" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B962" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C962">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="963" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A963" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B963" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C963">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="964" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A964" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B964" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C964">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="965" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A965" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B965" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C965">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="966" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A966" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B966" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C966">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="967" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A967" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C967">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="968" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A968" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C968">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="969" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A969" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B969" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C969">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="970" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A970" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B970" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C970">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="971" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A971" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B971" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C971">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="972" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A972" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B972" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C972">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="973" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A973" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B973" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C973">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:C1048576">

</xml_diff>